<commit_message>
[web] - support auto-search for chrome and firefox binary when the "default" or system-defined binary path cannot be found.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data-management/artifact/script/ManagedViaProjectProperties.xlsx
+++ b/examples/data-management/artifact/script/ManagedViaProjectProperties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lium183/projects/nexial/tutorials/examples/data-management/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8403B4-91DC-7641-A364-D9B95609FCB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D312F1-E8A0-7A46-8159-1C6A39A69DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="558">
   <si>
     <t>description</t>
   </si>
@@ -1878,6 +1878,27 @@
 C'mon in! The sale won't last forever!
 </t>
     </r>
+  </si>
+  <si>
+    <t>${MyTest.site.homepage}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Check out these great deals at </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>${MyTest.site.homepage}</t>
+    </r>
+  </si>
+  <si>
+    <t>PauseAfter()</t>
   </si>
 </sst>
 </file>
@@ -2034,7 +2055,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2162,6 +2183,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4509,9 +4534,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4673,9 +4698,15 @@
     <row r="6" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="B6" s="5"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="C6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>556</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -4690,14 +4721,22 @@
     <row r="7" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="C7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>555</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="22"/>
+      <c r="J7" s="22" t="s">
+        <v>557</v>
+      </c>
       <c r="K7" s="3"/>
       <c r="L7" s="15"/>
       <c r="M7" s="12"/>

</xml_diff>